<commit_message>
Final code changes on 22nd feb 2022
</commit_message>
<xml_diff>
--- a/MDSi/src/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/src/TestFiles/MDSiTestResult.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="14">
   <si>
     <t>FileName</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>72004073</t>
+  </si>
+  <si>
+    <t>32001322</t>
+  </si>
+  <si>
+    <t>32265125</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
changes of 2nd May 2022
</commit_message>
<xml_diff>
--- a/MDSi/src/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/src/TestFiles/MDSiTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>FileName</t>
   </si>
@@ -227,6 +227,42 @@
   </si>
   <si>
     <t>32376217</t>
+  </si>
+  <si>
+    <t>32376658</t>
+  </si>
+  <si>
+    <t>32376659</t>
+  </si>
+  <si>
+    <t>32376660</t>
+  </si>
+  <si>
+    <t>32378671</t>
+  </si>
+  <si>
+    <t>32378672</t>
+  </si>
+  <si>
+    <t>32378673</t>
+  </si>
+  <si>
+    <t>32378878</t>
+  </si>
+  <si>
+    <t>32378879</t>
+  </si>
+  <si>
+    <t>32378880</t>
+  </si>
+  <si>
+    <t>32378887</t>
+  </si>
+  <si>
+    <t>32378888</t>
+  </si>
+  <si>
+    <t>32378889</t>
   </si>
 </sst>
 </file>
@@ -603,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -635,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -649,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -663,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>